<commit_message>
v2.1 - bug fixes and design update
</commit_message>
<xml_diff>
--- a/hardware/control_board/BORC_v2_control_board__BOM.xlsx
+++ b/hardware/control_board/BORC_v2_control_board__BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AKstudios\Documents\GitHub\berg-lab BORC\hardware\control_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39B91E8-EF47-4FA6-B16E-3D7DA21E53AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16DDF58-7B5B-46F5-9C2A-7D10D5950404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="0" windowWidth="19200" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="198">
   <si>
     <t>Parts</t>
   </si>
@@ -55,21 +55,12 @@
     <t>0.1uF</t>
   </si>
   <si>
-    <t>GRM155R71C104KA88J</t>
-  </si>
-  <si>
     <t>C1, C7</t>
   </si>
   <si>
     <t>0.33µF</t>
   </si>
   <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>1.69M</t>
-  </si>
-  <si>
     <t>RC0402FR-7W10KL</t>
   </si>
   <si>
@@ -88,21 +79,12 @@
     <t>100uF</t>
   </si>
   <si>
-    <t>R2, R8, R15, R16, R19, R20, R21, R22, R23, R24, R25, R28, R29, R30, R35, R36, R37, R38, R44, R45, R46, R47, R49, R50</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
-    <t>R3, R5, R17</t>
-  </si>
-  <si>
     <t>10M</t>
   </si>
   <si>
-    <t>C15, C32, C33</t>
-  </si>
-  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -127,30 +109,12 @@
     <t>R13, R14</t>
   </si>
   <si>
-    <t>R34</t>
-  </si>
-  <si>
     <t>R9, R10</t>
   </si>
   <si>
     <t>4.7K</t>
   </si>
   <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>470k</t>
-  </si>
-  <si>
-    <t>C31</t>
-  </si>
-  <si>
-    <t>470nF</t>
-  </si>
-  <si>
-    <t>47uF</t>
-  </si>
-  <si>
     <t>R11, R12</t>
   </si>
   <si>
@@ -262,9 +226,6 @@
     <t>U5</t>
   </si>
   <si>
-    <t>RPM5.0-3.0</t>
-  </si>
-  <si>
     <t>J5</t>
   </si>
   <si>
@@ -283,30 +244,9 @@
     <t>SW1</t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>SRN5040TA-2R2M</t>
-  </si>
-  <si>
-    <t>Q5, Q7, Q11</t>
-  </si>
-  <si>
     <t>SSM3J374R,LF</t>
   </si>
   <si>
-    <t>Q6</t>
-  </si>
-  <si>
-    <t>SSM3K376R,LF</t>
-  </si>
-  <si>
-    <t>U12</t>
-  </si>
-  <si>
-    <t>SY6982C</t>
-  </si>
-  <si>
     <t>Q1, Q4, Q16</t>
   </si>
   <si>
@@ -361,12 +301,6 @@
     <t>0.33 µF ±10% 50V Ceramic Capacitor X7R 0805 (2012 Metric)</t>
   </si>
   <si>
-    <t>RC0402FR-071M69L</t>
-  </si>
-  <si>
-    <t>1.69 MOhms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Moisture Resistant Thick Film</t>
-  </si>
-  <si>
     <t>10 Ohms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Moisture Resistant Thick Film</t>
   </si>
   <si>
@@ -385,15 +319,6 @@
     <t>100 µF 25 V Aluminum - Polymer Capacitors Radial, Can - SMD 36mOhm 2000 Hrs @ 125°C</t>
   </si>
   <si>
-    <t>C28, C29</t>
-  </si>
-  <si>
-    <t>GRM21BR61A476ME15K</t>
-  </si>
-  <si>
-    <t>47 µF ±20% 10V Ceramic Capacitor X5R 0805 (2012 Metric)</t>
-  </si>
-  <si>
     <t>10 kOhms ±1% 0.125W, 1/8W Chip Resistor 0402 (1005 Metric) Moisture Resistant Thick Film</t>
   </si>
   <si>
@@ -409,9 +334,6 @@
     <t>10 µF ±10% 50V Ceramic Capacitor X5R 0805 (2012 Metric)</t>
   </si>
   <si>
-    <t>0.1 µF ±10% 16V Ceramic Capacitor X7R 0402 (1005 Metric)</t>
-  </si>
-  <si>
     <t>CSTNE16M0V530000R0</t>
   </si>
   <si>
@@ -442,33 +364,12 @@
     <t>27 Ohms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Moisture Resistant Thick Film</t>
   </si>
   <si>
-    <t>R1, R6, R7, R40, R48</t>
-  </si>
-  <si>
-    <t>RC0402FR-13330RL</t>
-  </si>
-  <si>
-    <t>330 Ohms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Thick Film</t>
-  </si>
-  <si>
     <t>RC0402FR-074K7L</t>
   </si>
   <si>
     <t>4.7 kOhms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Moisture Resistant Thick Film</t>
   </si>
   <si>
-    <t>RC0402FR-13470KL</t>
-  </si>
-  <si>
-    <t>470 kOhms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Thick Film</t>
-  </si>
-  <si>
-    <t>GRT155R61C474KE01D</t>
-  </si>
-  <si>
-    <t>0.47 µF ±10% 16V Ceramic Capacitor X5R 0402 (1005 Metric)</t>
-  </si>
-  <si>
     <t>RC0402FR-135K1L</t>
   </si>
   <si>
@@ -592,15 +493,6 @@
     <t>Red 631nm LED Indication - Discrete 2.1V 0402 (1005 Metric)</t>
   </si>
   <si>
-    <t>Recom Power</t>
-  </si>
-  <si>
-    <t>Non-Isolated PoL Module DC DC Converter 1 Output 5V 3A 3V - 17V Input</t>
-  </si>
-  <si>
-    <t>5V 3A</t>
-  </si>
-  <si>
     <t>S2B-XH-A</t>
   </si>
   <si>
@@ -637,33 +529,15 @@
     <t>SPST-NO 50mA 32V</t>
   </si>
   <si>
-    <t>2.2 µH Semi-Shielded Drum Core, Wirewound Inductor 3.8 A 21mOhm Nonstandard</t>
-  </si>
-  <si>
-    <t>2.2uH 3.8A 5x5mm</t>
-  </si>
-  <si>
     <t>P-Channel 30 V 4A (Ta) 1W (Ta) Surface Mount SOT-23F</t>
   </si>
   <si>
     <t>Toshiba Semiconductor and Storage</t>
   </si>
   <si>
-    <t>N-Channel 30 V 4A (Ta) 2W (Ta) Surface Mount SOT-23F</t>
-  </si>
-  <si>
     <t>P-CH 30V 4A SOT23F</t>
   </si>
   <si>
-    <t>N-CH 30V 4A SOT23F</t>
-  </si>
-  <si>
-    <t>Silergy</t>
-  </si>
-  <si>
-    <t>High Efficiency, 2A, Two-Cell Boost Li-Ion Battery Charger</t>
-  </si>
-  <si>
     <t>Bipolar (BJT) Transistor NPN 40 V 200 mA 300MHz 200 mW Surface Mount UMT3</t>
   </si>
   <si>
@@ -688,10 +562,58 @@
     <t>Yellow 592nm LED Indication - Discrete 1.9V 0402 (1005 Metric)</t>
   </si>
   <si>
-    <t>C2, C3, C4, C5, C6, C8, C9, C10, C11, C12, C13, C18, C21, C23, C25, C26, C27</t>
-  </si>
-  <si>
-    <t>C24, C30</t>
+    <t>C2, C3, C4, C6, C9, C10, C11, C12, C13, C18, C21, C25, C26</t>
+  </si>
+  <si>
+    <t>R2, R8, R15, R16, R19, R20, R21, R22, R23, R24, R25, R28, R29, R30, R31, R32, R33, R35, R44, R45, R46, R47, R49, R50</t>
+  </si>
+  <si>
+    <t>R3, R5, R17, R18</t>
+  </si>
+  <si>
+    <t>R1, R6, R7, R27, R36, R40, R48</t>
+  </si>
+  <si>
+    <t>Q1, Q2, Q5, Q7, Q11</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C8, C20, C22, C24, C30, C32, C33</t>
+  </si>
+  <si>
+    <t>MBR260HW</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>SMC Diode Solutions</t>
+  </si>
+  <si>
+    <t>60V, 2A</t>
+  </si>
+  <si>
+    <t>Diode 60 V 2A Surface Mount SOD-123</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>MCP73833T-AMI/MF</t>
+  </si>
+  <si>
+    <t>Charger IC Lithium Ion/Polymer 10-DFN (3x3)</t>
+  </si>
+  <si>
+    <t>Pololu Corporation</t>
+  </si>
+  <si>
+    <t>Non-Isolated PoL Module DC DC Converter 1 Output 5V 3.5A 1.3V - 5V Input</t>
+  </si>
+  <si>
+    <t>U3V40F5</t>
   </si>
 </sst>
 </file>
@@ -849,7 +771,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1032,12 +954,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1217,7 +1133,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1234,14 +1150,17 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1598,11 +1517,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1626,7 +1543,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>3</v>
@@ -1635,7 +1552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1646,10 +1563,10 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1660,16 +1577,16 @@
         <v>7</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -1680,516 +1597,516 @@
         <v>10</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>103</v>
+        <v>86</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>222</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="8" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>180</v>
       </c>
       <c r="B5" s="7">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>108</v>
+        <v>89</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="7">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>111</v>
+        <v>89</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="F7" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>100</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="7">
+        <v>24</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" s="7">
+        <v>4</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" s="7">
+        <v>6</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" s="7">
+        <v>7</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="7">
+      <c r="F15" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="7">
         <v>2</v>
       </c>
-      <c r="C8" s="7">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="7">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7">
-        <v>100</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="7">
-        <v>1</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B11" s="7">
-        <v>2</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="C16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="7">
-        <v>24</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="7">
-        <v>3</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="7">
-        <v>3</v>
-      </c>
-      <c r="C14" s="7" t="s">
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="B15" s="7">
-        <v>2</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="B17" s="7">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7">
+        <v>220</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="B16" s="7">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B17" s="7">
-        <v>5</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="B18" s="7">
         <v>2</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>32</v>
+      <c r="C18" s="7">
+        <v>27</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B19" s="7">
-        <v>1</v>
-      </c>
-      <c r="C19" s="7">
-        <v>220</v>
+        <v>2</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B20" s="7">
         <v>2</v>
       </c>
-      <c r="C20" s="7">
-        <v>27</v>
+      <c r="C20" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="7">
-        <v>1</v>
-      </c>
-      <c r="C21" s="7">
-        <v>330</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="F21" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C23" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="B24" s="7">
+        <v>1</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="7">
-        <v>1</v>
-      </c>
-      <c r="C24" s="7" t="s">
+      <c r="B25" s="7">
+        <v>1</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+      <c r="D25" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="7">
-        <v>2</v>
-      </c>
-      <c r="C25" s="7" t="s">
+      <c r="D26" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+      <c r="F26" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="7">
-        <v>1</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="B27" s="7">
+        <v>3</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="E26" s="7" t="s">
+      <c r="D27" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+      <c r="B28" s="7">
+        <v>1</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="7">
-        <v>1</v>
-      </c>
-      <c r="C27" s="7" t="s">
+      <c r="D28" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="7">
-        <v>6</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+      <c r="D29" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="7">
-        <v>1</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>159</v>
-      </c>
       <c r="F29" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>52</v>
       </c>
@@ -2200,16 +2117,16 @@
         <v>53</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>53</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>54</v>
       </c>
@@ -2220,473 +2137,353 @@
         <v>55</v>
       </c>
       <c r="D31" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B32" s="7">
+        <v>1</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="7">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="7">
+        <v>1</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B35" s="7">
+        <v>1</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="7">
+        <v>1</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="7">
+        <v>1</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="7">
+        <v>1</v>
+      </c>
+      <c r="C38" s="7">
+        <v>4012</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="7">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="7">
+        <v>2</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="7">
+        <v>1</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="7">
+        <v>1</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="7">
+        <v>3</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F43" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="7" t="s">
+    </row>
+    <row r="44" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="7">
+        <v>1</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E44" s="7" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="7">
-        <v>3</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F32" s="7" t="s">
+      <c r="F44" s="7" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="7">
-        <v>1</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F33" s="7" t="s">
+    <row r="45" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B45" s="7">
+        <v>5</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="7">
-        <v>1</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" s="7">
-        <v>1</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="7">
-        <v>1</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="7">
-        <v>1</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="7">
-        <v>1</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B39" s="7">
-        <v>1</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="7">
-        <v>1</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+    <row r="46" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="B41" s="7">
-        <v>1</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" s="7">
-        <v>2</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B43" s="7">
-        <v>1</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" s="7">
-        <v>1</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" s="7">
-        <v>1</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="B46" s="7">
         <v>3</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>85</v>
+        <v>174</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B47" s="7">
         <v>1</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B48" s="7">
         <v>1</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>206</v>
+        <v>79</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B49" s="7">
-        <v>3</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B50" s="7">
-        <v>1</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B51" s="7">
-        <v>1</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B52" s="7">
-        <v>3</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B53" s="7">
-        <v>1</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B54" s="7">
-        <v>1</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>